<commit_message>
- zmiany i udoskonalenie pliku exel z podzespolami - calkowite przerobienie schematu zgodnie z sztuka z filmu nr2 - zmiana procka i podlaczenie go - zmiana transcivera i podlaczenie go
</commit_message>
<xml_diff>
--- a/Kosztorys/Zestawienie i kosztorys komponentow.xlsx
+++ b/Kosztorys/Zestawienie i kosztorys komponentow.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t xml:space="preserve">Nazwa </t>
   </si>
@@ -22,7 +22,13 @@
     <t>Cena [1szt]</t>
   </si>
   <si>
-    <t>Cena [10szt]</t>
+    <t>Cena [1szt przy zakupie 10szt]</t>
+  </si>
+  <si>
+    <t>Cena[10szt]</t>
+  </si>
+  <si>
+    <t>Cena [1szt przy zakupie 100szt]</t>
   </si>
   <si>
     <t>Cena [100szt]</t>
@@ -31,6 +37,15 @@
     <t>Link</t>
   </si>
   <si>
+    <t xml:space="preserve">Procesor </t>
+  </si>
+  <si>
+    <t>STM</t>
+  </si>
+  <si>
+    <t>https://www.mouser.pl/ProductDetail/STMicroelectronics/STM32F030K6T6?qs=eyrSuY1LhL2nYlb0JDdrAA%3D%3D</t>
+  </si>
+  <si>
     <t>Transoptor</t>
   </si>
   <si>
@@ -88,10 +103,40 @@
     <t>Wyświetlacz</t>
   </si>
   <si>
+    <t>https://www.tme.eu/pl/details/eadogs164n-a/wyswietlacze-lcd-alfanumeryczne/display-visions/ea-dogs164n-a/?fbclid=IwAR1gLK8HvjWFd01Zgx7vMY-rJ60BwQ1qTm_Hiv7KvT-JQg85gzyA3S0SR8U</t>
+  </si>
+  <si>
     <t>Transciver</t>
   </si>
   <si>
+    <t>https://botland.com.pl/moduly-wifi-i-bt-esp32/10018-uklad-wifi-bluetooth-ble-esp-wroom-32-smd-27v-36v-5904422338718.html</t>
+  </si>
+  <si>
     <t>Moduł programatora</t>
+  </si>
+  <si>
+    <t>listwa goldpin do programatora</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/pl/details/20021111-00010t4lf/listwy-i-gniazda-kolkowe/amphenol-communications-solutions/</t>
+  </si>
+  <si>
+    <t>Suma dla 1szt</t>
+  </si>
+  <si>
+    <t>Suma dla 10szt</t>
+  </si>
+  <si>
+    <t>Suma dla 100szt</t>
+  </si>
+  <si>
+    <t>cena 1 szt przy zrobieniu 1</t>
+  </si>
+  <si>
+    <t>cena 1 szt przy zrobieniu 10</t>
+  </si>
+  <si>
+    <t>cena 1 szt przy zrobieniu 100</t>
   </si>
 </sst>
 </file>
@@ -101,7 +146,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$zł-415]"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -122,13 +167,25 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -137,23 +194,33 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0" applyFill="1" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -372,6 +439,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="15.5"/>
     <col customWidth="1" min="2" max="2" width="19.38"/>
+    <col customWidth="1" min="4" max="4" width="25.88"/>
+    <col customWidth="1" min="6" max="6" width="26.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -381,182 +450,376 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3">
-        <v>5.39</v>
-      </c>
-      <c r="D2" s="3">
-        <v>3.52</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2.28</v>
-      </c>
-      <c r="F2" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4">
+        <v>11.21</v>
+      </c>
+      <c r="D2" s="4">
+        <v>10.1</v>
+      </c>
+      <c r="E2" s="4">
+        <f t="shared" ref="E2:E11" si="1">10*D2</f>
+        <v>101</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8.13</v>
+      </c>
+      <c r="G2" s="4">
+        <f t="shared" ref="G2:G11" si="2">100*F2</f>
+        <v>813</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3">
-        <v>11.06</v>
-      </c>
-      <c r="D3" s="3">
-        <v>10.39</v>
-      </c>
-      <c r="E3" s="3">
-        <v>9.24</v>
-      </c>
-      <c r="F3" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4">
+        <v>5.39</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3.52</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" si="1"/>
+        <v>35.2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>2.28</v>
+      </c>
+      <c r="G3" s="6">
+        <f t="shared" si="2"/>
+        <v>228</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.48</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.39</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.21</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="C4" s="4">
+        <v>11.06</v>
+      </c>
+      <c r="D4" s="4">
+        <v>10.39</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="1"/>
+        <v>103.9</v>
+      </c>
+      <c r="F4" s="4">
+        <v>9.24</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" si="2"/>
+        <v>924</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="3">
-        <v>8.37</v>
-      </c>
-      <c r="D5" s="3">
-        <v>5.29</v>
-      </c>
-      <c r="E5" s="3">
-        <v>5.15</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.48</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.39</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="1"/>
+        <v>3.9</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3">
-        <v>5.0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>5.0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>5.0</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="C6" s="4">
+        <v>8.37</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5.29</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="1"/>
+        <v>52.9</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5.15</v>
+      </c>
+      <c r="G6" s="6">
+        <f t="shared" si="2"/>
+        <v>515</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="3">
-        <v>2.79</v>
-      </c>
-      <c r="D7" s="3">
-        <v>2.67</v>
-      </c>
-      <c r="E7" s="3">
-        <v>2.23</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="C7" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="F7" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2.79</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2.67</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="1"/>
+        <v>26.7</v>
+      </c>
+      <c r="F8" s="4">
+        <v>2.23</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" si="2"/>
+        <v>223</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="C9" s="4">
+        <v>75.0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>55.0</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="1"/>
+        <v>550</v>
+      </c>
+      <c r="F9" s="4">
+        <v>50.0</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="2"/>
+        <v>5000</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="4">
+        <v>38.0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>38.0</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="1"/>
+        <v>380</v>
+      </c>
+      <c r="F10" s="4">
+        <v>38.0</v>
+      </c>
+      <c r="G10" s="6">
+        <f t="shared" si="2"/>
+        <v>3800</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11">
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="F11" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12">
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="8">
+        <f>SUM(C2:C11)</f>
+        <v>159.9</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="8">
+        <f>SUM(E2:E11)</f>
+        <v>1329.6</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="8">
+        <f>SUM(G2:G11)</f>
+        <v>12224</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="8">
+        <f>B14</f>
+        <v>159.9</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="8">
+        <f>B15/10</f>
+        <v>132.96</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="9">
+        <f>B16/100</f>
+        <v>122.24</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2"/>
-    <hyperlink r:id="rId2" ref="F3"/>
-    <hyperlink r:id="rId3" ref="F4"/>
-    <hyperlink r:id="rId4" ref="F5"/>
-    <hyperlink r:id="rId5" ref="F6"/>
-    <hyperlink r:id="rId6" ref="F7"/>
+    <hyperlink r:id="rId1" ref="H2"/>
+    <hyperlink r:id="rId2" ref="H3"/>
+    <hyperlink r:id="rId3" ref="H4"/>
+    <hyperlink r:id="rId4" ref="H5"/>
+    <hyperlink r:id="rId5" ref="H6"/>
+    <hyperlink r:id="rId6" ref="H7"/>
+    <hyperlink r:id="rId7" ref="H8"/>
+    <hyperlink r:id="rId8" ref="H9"/>
+    <hyperlink r:id="rId9" ref="H10"/>
+    <hyperlink r:id="rId10" ref="H11"/>
   </hyperlinks>
-  <drawing r:id="rId7"/>
+  <drawing r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>